<commit_message>
amaze back end template UI
</commit_message>
<xml_diff>
--- a/template/auto_gene/user/gene_site/_gene_/templates/schema.xlsx
+++ b/template/auto_gene/user/gene_site/_gene_/templates/schema.xlsx
@@ -1,7 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr date1904="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
@@ -9,12 +8,13 @@
     <sheet name="admin" sheetId="1" r:id="rId4"/>
     <sheet name="table" sheetId="2" r:id="rId5"/>
     <sheet name="default_fields" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
   <si>
     <t>name</t>
   </si>
@@ -133,6 +133,33 @@
     <t>1:普通读者；2:图书管理员；3:系统管理员</t>
   </si>
   <si>
+    <t>birth</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>出生</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>varchar(1024)</t>
+  </si>
+  <si>
+    <t>简介</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>varchar(200)</t>
+  </si>
+  <si>
+    <t>地址</t>
+  </si>
+  <si>
     <t>varchar(500)</t>
   </si>
   <si>
@@ -145,39 +172,12 @@
     <t>summary</t>
   </si>
   <si>
-    <t>varchar(1024)</t>
-  </si>
-  <si>
-    <t>简介</t>
-  </si>
-  <si>
     <t>amount</t>
   </si>
   <si>
     <t>数量</t>
   </si>
   <si>
-    <t>birth</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>出生</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>varchar(200)</t>
-  </si>
-  <si>
-    <t>地址</t>
-  </si>
-  <si>
     <t>user_book</t>
   </si>
   <si>
@@ -227,6 +227,15 @@
   </si>
   <si>
     <t>publish_date</t>
+  </si>
+  <si>
+    <t>article</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
   <si>
     <t>PK</t>
@@ -298,12 +307,12 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Verdana"/>
+      <name val="宋体"/>
     </font>
     <font>
       <sz val="15"/>
       <color indexed="8"/>
-      <name val="Verdana"/>
+      <name val="宋体"/>
     </font>
     <font>
       <b val="1"/>
@@ -343,7 +352,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -363,6 +372,95 @@
       </top>
       <bottom style="thin">
         <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -392,6 +490,43 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="10"/>
       </left>
       <right style="thin">
@@ -403,42 +538,169 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -446,11 +708,44 @@
     <xf numFmtId="1" fontId="5" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1704,176 +1999,125 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="7.875" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.125" style="1" customWidth="1"/>
-    <col min="7" max="256" width="9" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1"/>
+    <col min="6" max="256" width="7.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.35" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" s="4"/>
+      <c r="D1" s="3"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
     </row>
     <row r="2" ht="20.35" customHeight="1">
-      <c r="A2" t="s" s="2">
+      <c r="A2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="6">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="6">
         <v>5</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" ht="20.35" customHeight="1">
-      <c r="A3" t="s" s="2">
+      <c r="A3" t="s" s="9">
         <v>6</v>
       </c>
-      <c r="B3" t="s" s="3">
+      <c r="B3" t="s" s="10">
         <v>7</v>
       </c>
-      <c r="C3" t="s" s="3">
+      <c r="C3" t="s" s="10">
         <v>8</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" t="s" s="2">
+      <c r="A4" t="s" s="9">
         <v>9</v>
       </c>
-      <c r="B4" t="s" s="3">
+      <c r="B4" t="s" s="10">
         <v>10</v>
       </c>
-      <c r="C4" t="s" s="3">
+      <c r="C4" t="s" s="10">
         <v>10</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" t="s" s="2">
+      <c r="A5" t="s" s="9">
         <v>11</v>
       </c>
-      <c r="B5" t="s" s="3">
+      <c r="B5" t="s" s="10">
         <v>12</v>
       </c>
-      <c r="C5" t="s" s="3">
+      <c r="C5" t="s" s="10">
         <v>12</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" s="5"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" s="5"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" ht="20.35" customHeight="1">
-      <c r="A12" s="5"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" s="5"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="5"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1887,848 +2131,856 @@
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="1" style="6" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="6" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="6" customWidth="1"/>
-    <col min="5" max="5" width="12.25" style="6" customWidth="1"/>
-    <col min="6" max="6" width="14" style="6" customWidth="1"/>
-    <col min="7" max="7" width="7.25" style="6" customWidth="1"/>
-    <col min="8" max="8" width="7.25" style="6" customWidth="1"/>
-    <col min="9" max="9" width="14" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14" style="6" customWidth="1"/>
-    <col min="11" max="256" width="12.25" style="6" customWidth="1"/>
+    <col min="1" max="1" width="1" style="16" customWidth="1"/>
+    <col min="2" max="2" width="10.75" style="16" customWidth="1"/>
+    <col min="3" max="3" width="10.75" style="16" customWidth="1"/>
+    <col min="4" max="4" width="10.75" style="16" customWidth="1"/>
+    <col min="5" max="5" width="10.75" style="16" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="16" customWidth="1"/>
+    <col min="7" max="7" width="6.375" style="16" customWidth="1"/>
+    <col min="8" max="8" width="6.375" style="16" customWidth="1"/>
+    <col min="9" max="9" width="12.25" style="16" customWidth="1"/>
+    <col min="10" max="10" width="12.25" style="16" customWidth="1"/>
+    <col min="11" max="256" width="10.75" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.55" customHeight="1">
-      <c r="A1" s="7"/>
-      <c r="B1" t="s" s="8">
+      <c r="A1" s="17"/>
+      <c r="B1" t="s" s="18">
         <v>13</v>
       </c>
-      <c r="C1" t="s" s="8">
+      <c r="C1" t="s" s="18">
         <v>14</v>
       </c>
-      <c r="D1" t="s" s="8">
+      <c r="D1" t="s" s="18">
         <v>15</v>
       </c>
-      <c r="E1" t="s" s="8">
+      <c r="E1" t="s" s="18">
         <v>16</v>
       </c>
-      <c r="F1" t="s" s="8">
+      <c r="F1" t="s" s="18">
         <v>1</v>
       </c>
-      <c r="G1" t="s" s="8">
+      <c r="G1" t="s" s="18">
         <v>17</v>
       </c>
-      <c r="H1" t="s" s="8">
+      <c r="H1" t="s" s="18">
         <v>18</v>
       </c>
-      <c r="I1" t="s" s="8">
+      <c r="I1" t="s" s="18">
         <v>19</v>
       </c>
-      <c r="J1" t="s" s="8">
+      <c r="J1" t="s" s="18">
         <v>20</v>
       </c>
     </row>
     <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" s="9"/>
+      <c r="A2" s="19"/>
       <c r="B2" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="20">
         <v>0</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="21">
         <v>21</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" t="s" s="21">
         <v>22</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="F2" t="s" s="21">
         <v>23</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" ht="20.35" customHeight="1">
-      <c r="A3" s="9"/>
+      <c r="A3" s="19"/>
       <c r="B3" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="C3" t="s" s="10">
+      <c r="C3" t="s" s="24">
         <v>24</v>
       </c>
-      <c r="D3" t="s" s="10">
+      <c r="D3" t="s" s="24">
         <v>25</v>
       </c>
-      <c r="E3" t="s" s="10">
+      <c r="E3" t="s" s="24">
         <v>22</v>
       </c>
-      <c r="F3" t="s" s="10">
+      <c r="F3" t="s" s="24">
         <v>26</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" s="9"/>
+      <c r="A4" s="19"/>
       <c r="B4" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="C4" t="s" s="3">
+      <c r="C4" t="s" s="20">
         <v>27</v>
       </c>
-      <c r="D4" t="s" s="3">
+      <c r="D4" t="s" s="21">
         <v>28</v>
       </c>
-      <c r="E4" t="s" s="3">
+      <c r="E4" t="s" s="21">
         <v>22</v>
       </c>
-      <c r="F4" t="s" s="3">
+      <c r="F4" t="s" s="21">
         <v>29</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="23"/>
     </row>
     <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" s="9"/>
+      <c r="A5" s="19"/>
       <c r="B5" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="C5" t="s" s="10">
+      <c r="C5" t="s" s="24">
         <v>30</v>
       </c>
-      <c r="D5" t="s" s="10">
+      <c r="D5" t="s" s="24">
         <v>31</v>
       </c>
-      <c r="E5" t="s" s="10">
+      <c r="E5" t="s" s="24">
         <v>32</v>
       </c>
-      <c r="F5" t="s" s="10">
+      <c r="F5" t="s" s="24">
         <v>33</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
     </row>
     <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" s="9"/>
+      <c r="A6" s="19"/>
       <c r="B6" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="C6" t="s" s="3">
+      <c r="C6" t="s" s="20">
         <v>34</v>
       </c>
-      <c r="D6" t="s" s="3">
+      <c r="D6" t="s" s="21">
         <v>21</v>
       </c>
-      <c r="E6" t="s" s="3">
+      <c r="E6" t="s" s="21">
         <v>32</v>
       </c>
-      <c r="F6" t="s" s="3">
+      <c r="F6" t="s" s="21">
         <v>35</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" ht="32.6" customHeight="1">
-      <c r="A7" s="9"/>
+      <c r="A7" s="19"/>
       <c r="B7" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="C7" t="s" s="10">
+      <c r="C7" t="s" s="24">
         <v>36</v>
       </c>
-      <c r="D7" t="s" s="10">
+      <c r="D7" t="s" s="24">
         <v>31</v>
       </c>
-      <c r="E7" t="s" s="10">
+      <c r="E7" t="s" s="24">
         <v>22</v>
       </c>
-      <c r="F7" t="s" s="10">
+      <c r="F7" t="s" s="24">
         <v>37</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="24">
         <v>1</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" t="s" s="10">
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" t="s" s="24">
         <v>38</v>
       </c>
     </row>
     <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="23"/>
     </row>
     <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" s="9"/>
+      <c r="A9" s="19"/>
       <c r="B9" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s" s="24">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s" s="24">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s" s="24">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s" s="24">
+        <v>23</v>
+      </c>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+    </row>
+    <row r="10" ht="20.35" customHeight="1">
+      <c r="A10" s="19"/>
+      <c r="B10" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s" s="20">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s" s="21">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s" s="21">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s" s="21">
+        <v>41</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="23"/>
+    </row>
+    <row r="11" ht="20.35" customHeight="1">
+      <c r="A11" s="19"/>
+      <c r="B11" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s" s="24">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s" s="24">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s" s="24">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s" s="24">
+        <v>44</v>
+      </c>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+    </row>
+    <row r="12" ht="20.35" customHeight="1">
+      <c r="A12" s="19"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="23"/>
+    </row>
+    <row r="13" ht="20.35" customHeight="1">
+      <c r="A13" s="19"/>
+      <c r="B13" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s" s="24">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s" s="24">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s" s="24">
+        <v>22</v>
+      </c>
+      <c r="F13" t="s" s="24">
+        <v>10</v>
+      </c>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+    </row>
+    <row r="14" ht="20.35" customHeight="1">
+      <c r="A14" s="19"/>
+      <c r="B14" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s" s="20">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s" s="21">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s" s="21">
+        <v>22</v>
+      </c>
+      <c r="F14" t="s" s="21">
+        <v>47</v>
+      </c>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="23"/>
+    </row>
+    <row r="15" ht="20.35" customHeight="1">
+      <c r="A15" s="19"/>
+      <c r="B15" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s" s="24">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s" s="24">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s" s="24">
+        <v>22</v>
+      </c>
+      <c r="F15" t="s" s="24">
+        <v>35</v>
+      </c>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+    </row>
+    <row r="16" ht="20.35" customHeight="1">
+      <c r="A16" s="12"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="23"/>
+    </row>
+    <row r="17" ht="20.35" customHeight="1">
+      <c r="A17" s="19"/>
+      <c r="B17" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="C9" t="s" s="10">
+      <c r="C17" t="s" s="24">
         <v>0</v>
       </c>
-      <c r="D9" t="s" s="10">
-        <v>39</v>
-      </c>
-      <c r="E9" t="s" s="10">
+      <c r="D17" t="s" s="24">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s" s="24">
         <v>22</v>
       </c>
-      <c r="F9" t="s" s="10">
-        <v>40</v>
-      </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-    </row>
-    <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" t="s" s="2">
+      <c r="F17" t="s" s="24">
+        <v>49</v>
+      </c>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+    </row>
+    <row r="18" ht="20.35" customHeight="1">
+      <c r="A18" s="19"/>
+      <c r="B18" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="C10" t="s" s="3">
+      <c r="C18" t="s" s="20">
         <v>9</v>
       </c>
-      <c r="D10" t="s" s="3">
-        <v>41</v>
-      </c>
-      <c r="E10" t="s" s="3">
+      <c r="D18" t="s" s="21">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s" s="21">
         <v>22</v>
       </c>
-      <c r="F10" t="s" s="3">
+      <c r="F18" t="s" s="21">
         <v>10</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" t="s" s="3">
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" t="s" s="21">
         <v>9</v>
       </c>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" s="9"/>
-      <c r="B11" t="s" s="2">
+      <c r="J18" s="23"/>
+    </row>
+    <row r="19" ht="20.35" customHeight="1">
+      <c r="A19" s="19"/>
+      <c r="B19" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="C11" t="s" s="10">
-        <v>42</v>
-      </c>
-      <c r="D11" t="s" s="10">
+      <c r="C19" t="s" s="24">
+        <v>51</v>
+      </c>
+      <c r="D19" t="s" s="24">
         <v>43</v>
       </c>
-      <c r="E11" t="s" s="10">
+      <c r="E19" t="s" s="24">
         <v>32</v>
       </c>
-      <c r="F11" t="s" s="10">
+      <c r="F19" t="s" s="24">
         <v>44</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-    </row>
-    <row r="12" ht="20.35" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" t="s" s="2">
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+    </row>
+    <row r="20" ht="20.35" customHeight="1">
+      <c r="A20" s="19"/>
+      <c r="B20" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="C12" t="s" s="3">
+      <c r="C20" t="s" s="20">
         <v>11</v>
       </c>
-      <c r="D12" t="s" s="3">
-        <v>41</v>
-      </c>
-      <c r="E12" t="s" s="3">
+      <c r="D20" t="s" s="21">
+        <v>50</v>
+      </c>
+      <c r="E20" t="s" s="21">
         <v>32</v>
       </c>
-      <c r="F12" t="s" s="3">
+      <c r="F20" t="s" s="21">
         <v>12</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" t="s" s="3">
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" t="s" s="21">
         <v>11</v>
       </c>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" s="9"/>
-      <c r="B13" t="s" s="2">
+      <c r="J20" s="23"/>
+    </row>
+    <row r="21" ht="20.35" customHeight="1">
+      <c r="A21" s="19"/>
+      <c r="B21" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="C13" t="s" s="10">
-        <v>45</v>
-      </c>
-      <c r="D13" t="s" s="10">
-        <v>41</v>
-      </c>
-      <c r="E13" t="s" s="10">
+      <c r="C21" t="s" s="24">
+        <v>52</v>
+      </c>
+      <c r="D21" t="s" s="24">
+        <v>50</v>
+      </c>
+      <c r="E21" t="s" s="24">
         <v>22</v>
       </c>
-      <c r="F13" t="s" s="10">
-        <v>46</v>
-      </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-    </row>
-    <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" s="9"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="9"/>
-      <c r="B15" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s" s="10">
-        <v>0</v>
-      </c>
-      <c r="D15" t="s" s="10">
-        <v>21</v>
-      </c>
-      <c r="E15" t="s" s="10">
-        <v>22</v>
-      </c>
-      <c r="F15" t="s" s="10">
-        <v>23</v>
-      </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-    </row>
-    <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" s="9"/>
-      <c r="B16" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s" s="3">
-        <v>47</v>
-      </c>
-      <c r="D16" t="s" s="3">
-        <v>48</v>
-      </c>
-      <c r="E16" t="s" s="3">
-        <v>32</v>
-      </c>
-      <c r="F16" t="s" s="3">
-        <v>49</v>
-      </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" s="9"/>
-      <c r="B17" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="C17" t="s" s="10">
-        <v>50</v>
-      </c>
-      <c r="D17" t="s" s="10">
-        <v>43</v>
-      </c>
-      <c r="E17" t="s" s="10">
-        <v>32</v>
-      </c>
-      <c r="F17" t="s" s="10">
-        <v>44</v>
-      </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-    </row>
-    <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" s="9"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" s="9"/>
-      <c r="B19" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="C19" t="s" s="10">
-        <v>0</v>
-      </c>
-      <c r="D19" t="s" s="10">
-        <v>21</v>
-      </c>
-      <c r="E19" t="s" s="10">
-        <v>22</v>
-      </c>
-      <c r="F19" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-    </row>
-    <row r="20" ht="20.35" customHeight="1">
-      <c r="A20" s="9"/>
-      <c r="B20" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="C20" t="s" s="3">
-        <v>51</v>
-      </c>
-      <c r="D20" t="s" s="3">
-        <v>52</v>
-      </c>
-      <c r="E20" t="s" s="3">
-        <v>22</v>
-      </c>
-      <c r="F20" t="s" s="3">
+      <c r="F21" t="s" s="24">
         <v>53</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" ht="20.35" customHeight="1">
-      <c r="A21" s="9"/>
-      <c r="B21" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="C21" t="s" s="10">
-        <v>34</v>
-      </c>
-      <c r="D21" t="s" s="10">
-        <v>52</v>
-      </c>
-      <c r="E21" t="s" s="10">
-        <v>22</v>
-      </c>
-      <c r="F21" t="s" s="10">
-        <v>35</v>
-      </c>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
     </row>
     <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" s="9"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="23"/>
     </row>
     <row r="23" ht="20.35" customHeight="1">
-      <c r="A23" s="9"/>
+      <c r="A23" s="19"/>
       <c r="B23" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="C23" t="s" s="10">
+      <c r="C23" t="s" s="24">
         <v>55</v>
       </c>
-      <c r="D23" t="s" s="10">
-        <v>41</v>
-      </c>
-      <c r="E23" t="s" s="10">
+      <c r="D23" t="s" s="24">
+        <v>50</v>
+      </c>
+      <c r="E23" t="s" s="24">
         <v>22</v>
       </c>
-      <c r="F23" t="s" s="10">
+      <c r="F23" t="s" s="24">
         <v>4</v>
       </c>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" t="s" s="10">
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" t="s" s="24">
         <v>3</v>
       </c>
-      <c r="J23" s="11"/>
+      <c r="J23" s="25"/>
     </row>
     <row r="24" ht="20.35" customHeight="1">
-      <c r="A24" s="9"/>
+      <c r="A24" s="19"/>
       <c r="B24" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="C24" t="s" s="3">
+      <c r="C24" t="s" s="20">
         <v>56</v>
       </c>
-      <c r="D24" t="s" s="3">
-        <v>41</v>
-      </c>
-      <c r="E24" t="s" s="3">
+      <c r="D24" t="s" s="21">
+        <v>50</v>
+      </c>
+      <c r="E24" t="s" s="21">
         <v>22</v>
       </c>
-      <c r="F24" t="s" s="3">
+      <c r="F24" t="s" s="21">
         <v>7</v>
       </c>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" t="s" s="3">
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" t="s" s="21">
         <v>6</v>
       </c>
-      <c r="J24" s="4"/>
+      <c r="J24" s="23"/>
     </row>
     <row r="25" ht="30.35" customHeight="1">
-      <c r="A25" s="9"/>
+      <c r="A25" s="19"/>
       <c r="B25" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="C25" t="s" s="10">
+      <c r="C25" t="s" s="24">
         <v>57</v>
       </c>
-      <c r="D25" t="s" s="10">
+      <c r="D25" t="s" s="24">
         <v>31</v>
       </c>
-      <c r="E25" t="s" s="10">
+      <c r="E25" t="s" s="24">
         <v>22</v>
       </c>
-      <c r="F25" t="s" s="10">
+      <c r="F25" t="s" s="24">
         <v>58</v>
       </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" t="s" s="10">
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" t="s" s="24">
         <v>59</v>
       </c>
     </row>
     <row r="26" ht="20.35" customHeight="1">
-      <c r="A26" s="9"/>
+      <c r="A26" s="19"/>
       <c r="B26" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="C26" t="s" s="3">
-        <v>45</v>
-      </c>
-      <c r="D26" t="s" s="3">
-        <v>41</v>
-      </c>
-      <c r="E26" t="s" s="3">
+      <c r="C26" t="s" s="20">
+        <v>52</v>
+      </c>
+      <c r="D26" t="s" s="21">
+        <v>50</v>
+      </c>
+      <c r="E26" t="s" s="21">
         <v>22</v>
       </c>
-      <c r="F26" t="s" s="3">
-        <v>46</v>
-      </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
+      <c r="F26" t="s" s="21">
+        <v>53</v>
+      </c>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="23"/>
     </row>
     <row r="27" ht="20.35" customHeight="1">
-      <c r="A27" s="9"/>
+      <c r="A27" s="19"/>
       <c r="B27" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="C27" t="s" s="10">
+      <c r="C27" t="s" s="24">
         <v>60</v>
       </c>
-      <c r="D27" t="s" s="10">
-        <v>48</v>
-      </c>
-      <c r="E27" t="s" s="10">
+      <c r="D27" t="s" s="24">
+        <v>40</v>
+      </c>
+      <c r="E27" t="s" s="24">
         <v>22</v>
       </c>
-      <c r="F27" t="s" s="10">
+      <c r="F27" t="s" s="24">
         <v>61</v>
       </c>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" t="s" s="10">
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" t="s" s="24">
         <v>61</v>
       </c>
     </row>
     <row r="28" ht="20.35" customHeight="1">
-      <c r="A28" s="9"/>
+      <c r="A28" s="19"/>
       <c r="B28" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="C28" t="s" s="3">
+      <c r="C28" t="s" s="20">
         <v>62</v>
       </c>
-      <c r="D28" t="s" s="3">
-        <v>48</v>
-      </c>
-      <c r="E28" t="s" s="3">
+      <c r="D28" t="s" s="21">
+        <v>40</v>
+      </c>
+      <c r="E28" t="s" s="21">
         <v>32</v>
       </c>
-      <c r="F28" t="s" s="3">
+      <c r="F28" t="s" s="21">
         <v>63</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" t="s" s="3">
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" t="s" s="27">
         <v>63</v>
       </c>
     </row>
     <row r="29" ht="20.35" customHeight="1">
-      <c r="A29" s="9"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" ht="20.35" customHeight="1">
-      <c r="A30" s="9"/>
+      <c r="A30" s="19"/>
       <c r="B30" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="C30" t="s" s="3">
+      <c r="C30" t="s" s="20">
         <v>56</v>
       </c>
-      <c r="D30" t="s" s="3">
-        <v>41</v>
-      </c>
-      <c r="E30" t="s" s="3">
+      <c r="D30" t="s" s="21">
+        <v>50</v>
+      </c>
+      <c r="E30" t="s" s="21">
         <v>22</v>
       </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" t="s" s="3">
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" t="s" s="21">
         <v>6</v>
       </c>
-      <c r="J30" s="4"/>
+      <c r="J30" s="23"/>
     </row>
     <row r="31" ht="20.35" customHeight="1">
-      <c r="A31" s="9"/>
+      <c r="A31" s="19"/>
       <c r="B31" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="C31" t="s" s="10">
+      <c r="C31" t="s" s="24">
         <v>65</v>
       </c>
-      <c r="D31" t="s" s="10">
-        <v>41</v>
-      </c>
-      <c r="E31" t="s" s="10">
+      <c r="D31" t="s" s="24">
+        <v>50</v>
+      </c>
+      <c r="E31" t="s" s="24">
         <v>22</v>
       </c>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" t="s" s="10">
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" t="s" s="24">
         <v>11</v>
       </c>
-      <c r="J31" s="11"/>
+      <c r="J31" s="25"/>
     </row>
     <row r="32" ht="20.35" customHeight="1">
-      <c r="A32" s="9"/>
+      <c r="A32" s="19"/>
       <c r="B32" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="C32" t="s" s="3">
+      <c r="C32" t="s" s="20">
         <v>66</v>
       </c>
-      <c r="D32" t="s" s="3">
-        <v>48</v>
-      </c>
-      <c r="E32" t="s" s="3">
+      <c r="D32" t="s" s="21">
+        <v>40</v>
+      </c>
+      <c r="E32" t="s" s="21">
         <v>22</v>
       </c>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="23"/>
     </row>
     <row r="33" ht="20.35" customHeight="1">
-      <c r="A33" s="9"/>
+      <c r="A33" s="19"/>
       <c r="B33" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="C33" t="s" s="10">
+      <c r="C33" t="s" s="24">
         <v>67</v>
       </c>
-      <c r="D33" t="s" s="10">
-        <v>48</v>
-      </c>
-      <c r="E33" t="s" s="10">
+      <c r="D33" t="s" s="24">
+        <v>40</v>
+      </c>
+      <c r="E33" t="s" s="24">
         <v>22</v>
       </c>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="25"/>
     </row>
     <row r="34" ht="20.35" customHeight="1">
-      <c r="A34" s="9"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="23"/>
     </row>
     <row r="35" ht="20.35" customHeight="1">
-      <c r="A35" s="9"/>
+      <c r="A35" s="19"/>
       <c r="B35" t="s" s="2">
         <v>68</v>
       </c>
-      <c r="C35" t="s" s="10">
+      <c r="C35" t="s" s="24">
         <v>56</v>
       </c>
-      <c r="D35" t="s" s="10">
-        <v>41</v>
-      </c>
-      <c r="E35" t="s" s="10">
+      <c r="D35" t="s" s="24">
+        <v>50</v>
+      </c>
+      <c r="E35" t="s" s="24">
         <v>22</v>
       </c>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" t="s" s="10">
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
+      <c r="I35" t="s" s="24">
         <v>6</v>
       </c>
-      <c r="J35" s="11"/>
+      <c r="J35" s="25"/>
     </row>
     <row r="36" ht="20.35" customHeight="1">
-      <c r="A36" s="9"/>
+      <c r="A36" s="19"/>
       <c r="B36" t="s" s="2">
         <v>68</v>
       </c>
-      <c r="C36" t="s" s="3">
+      <c r="C36" t="s" s="20">
         <v>69</v>
       </c>
-      <c r="D36" t="s" s="3">
-        <v>41</v>
-      </c>
-      <c r="E36" t="s" s="3">
+      <c r="D36" t="s" s="21">
+        <v>50</v>
+      </c>
+      <c r="E36" t="s" s="21">
         <v>22</v>
       </c>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" t="s" s="3">
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" t="s" s="21">
         <v>9</v>
       </c>
-      <c r="J36" s="4"/>
+      <c r="J36" s="23"/>
     </row>
     <row r="37" ht="20.35" customHeight="1">
-      <c r="A37" s="9"/>
+      <c r="A37" s="19"/>
       <c r="B37" t="s" s="2">
         <v>68</v>
       </c>
-      <c r="C37" t="s" s="10">
+      <c r="C37" t="s" s="24">
         <v>70</v>
       </c>
-      <c r="D37" t="s" s="10">
-        <v>48</v>
-      </c>
-      <c r="E37" t="s" s="10">
+      <c r="D37" t="s" s="24">
+        <v>40</v>
+      </c>
+      <c r="E37" t="s" s="24">
         <v>22</v>
       </c>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="25"/>
     </row>
     <row r="38" ht="20.35" customHeight="1">
-      <c r="A38" s="9"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
+      <c r="A38" s="19"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="23"/>
     </row>
     <row r="39" ht="20.35" customHeight="1">
-      <c r="A39" s="9"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
+      <c r="A39" s="19"/>
+      <c r="B39" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="C39" t="s" s="24">
+        <v>72</v>
+      </c>
+      <c r="D39" t="s" s="24">
+        <v>73</v>
+      </c>
+      <c r="E39" t="s" s="24">
+        <v>22</v>
+      </c>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
     </row>
     <row r="40" ht="20.35" customHeight="1">
-      <c r="A40" s="9"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
+      <c r="A40" s="19"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="23"/>
     </row>
     <row r="41" ht="20.35" customHeight="1">
-      <c r="A41" s="12"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
+      <c r="A41" s="28"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2742,211 +2994,306 @@
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="1" style="13" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="13" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="13" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="13" customWidth="1"/>
-    <col min="5" max="5" width="12.25" style="13" customWidth="1"/>
-    <col min="6" max="6" width="12.25" style="13" customWidth="1"/>
-    <col min="7" max="7" width="12.25" style="13" customWidth="1"/>
-    <col min="8" max="8" width="12.25" style="13" customWidth="1"/>
-    <col min="9" max="9" width="12.25" style="13" customWidth="1"/>
-    <col min="10" max="256" width="12.25" style="13" customWidth="1"/>
+    <col min="1" max="1" width="1" style="29" customWidth="1"/>
+    <col min="2" max="2" width="10.75" style="29" customWidth="1"/>
+    <col min="3" max="3" width="10.75" style="29" customWidth="1"/>
+    <col min="4" max="4" width="10.75" style="29" customWidth="1"/>
+    <col min="5" max="5" width="10.75" style="29" customWidth="1"/>
+    <col min="6" max="6" width="10.75" style="29" customWidth="1"/>
+    <col min="7" max="7" width="10.75" style="29" customWidth="1"/>
+    <col min="8" max="8" width="10.75" style="29" customWidth="1"/>
+    <col min="9" max="9" width="10.75" style="29" customWidth="1"/>
+    <col min="10" max="256" width="10.75" style="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.55" customHeight="1">
-      <c r="A1" s="7"/>
-      <c r="B1" t="s" s="8">
+      <c r="A1" s="17"/>
+      <c r="B1" t="s" s="18">
         <v>14</v>
       </c>
-      <c r="C1" t="s" s="8">
+      <c r="C1" t="s" s="18">
         <v>15</v>
       </c>
-      <c r="D1" t="s" s="8">
+      <c r="D1" t="s" s="18">
         <v>16</v>
       </c>
-      <c r="E1" t="s" s="8">
+      <c r="E1" t="s" s="18">
         <v>1</v>
       </c>
-      <c r="F1" t="s" s="8">
+      <c r="F1" t="s" s="18">
         <v>17</v>
       </c>
-      <c r="G1" t="s" s="8">
-        <v>71</v>
-      </c>
-      <c r="H1" t="s" s="8">
+      <c r="G1" t="s" s="18">
+        <v>74</v>
+      </c>
+      <c r="H1" t="s" s="18">
         <v>20</v>
       </c>
-      <c r="I1" t="s" s="8">
-        <v>72</v>
+      <c r="I1" t="s" s="18">
+        <v>75</v>
       </c>
     </row>
     <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" s="9"/>
+      <c r="A2" s="19"/>
       <c r="B2" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="C2" t="s" s="3">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s" s="3">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s" s="20">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s" s="21">
         <v>22</v>
       </c>
-      <c r="E2" t="s" s="3">
-        <v>74</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" t="s" s="3">
-        <v>75</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" t="s" s="3">
+      <c r="E2" t="s" s="21">
+        <v>77</v>
+      </c>
+      <c r="F2" s="22"/>
+      <c r="G2" t="s" s="21">
+        <v>78</v>
+      </c>
+      <c r="H2" s="22"/>
+      <c r="I2" t="s" s="30">
         <v>22</v>
       </c>
     </row>
     <row r="3" ht="20.35" customHeight="1">
-      <c r="A3" s="9"/>
+      <c r="A3" s="19"/>
       <c r="B3" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="C3" t="s" s="10">
-        <v>77</v>
-      </c>
-      <c r="D3" t="s" s="10">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s" s="24">
+        <v>80</v>
+      </c>
+      <c r="D3" t="s" s="24">
         <v>22</v>
       </c>
-      <c r="E3" t="s" s="10">
-        <v>78</v>
-      </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" t="s" s="3">
+      <c r="E3" t="s" s="24">
+        <v>81</v>
+      </c>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" t="s" s="31">
         <v>22</v>
       </c>
     </row>
     <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" s="9"/>
+      <c r="A4" s="19"/>
       <c r="B4" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="C4" t="s" s="3">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s" s="3">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s" s="20">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s" s="21">
         <v>32</v>
       </c>
-      <c r="E4" t="s" s="3">
+      <c r="E4" t="s" s="21">
+        <v>83</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" t="s" s="32">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" ht="20.35" customHeight="1">
+      <c r="A5" s="19"/>
+      <c r="B5" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="C5" t="s" s="24">
         <v>80</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" t="s" s="3">
+      <c r="D5" t="s" s="24">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s" s="24">
+        <v>85</v>
+      </c>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" t="s" s="31">
         <v>22</v>
       </c>
     </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" s="9"/>
-      <c r="B5" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="C5" t="s" s="10">
-        <v>77</v>
-      </c>
-      <c r="D5" t="s" s="10">
+    <row r="6" ht="20.35" customHeight="1">
+      <c r="A6" s="19"/>
+      <c r="B6" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="C6" t="s" s="20">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s" s="21">
         <v>32</v>
       </c>
-      <c r="E5" t="s" s="10">
-        <v>82</v>
-      </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" t="s" s="3">
+      <c r="E6" t="s" s="21">
+        <v>87</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" t="s" s="32">
         <v>22</v>
       </c>
     </row>
-    <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="C6" t="s" s="3">
-        <v>41</v>
-      </c>
-      <c r="D6" t="s" s="3">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s" s="3">
-        <v>84</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" t="s" s="3">
+    <row r="7" ht="42.6" customHeight="1">
+      <c r="A7" s="19"/>
+      <c r="B7" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="C7" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s" s="24">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" ht="42.6" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="C7" t="s" s="10">
-        <v>31</v>
-      </c>
-      <c r="D7" t="s" s="10">
+      <c r="E7" t="s" s="24">
+        <v>58</v>
+      </c>
+      <c r="F7" s="24">
+        <v>1</v>
+      </c>
+      <c r="G7" s="25"/>
+      <c r="H7" t="s" s="24">
+        <v>89</v>
+      </c>
+      <c r="I7" t="s" s="31">
         <v>22</v>
       </c>
-      <c r="E7" t="s" s="10">
-        <v>58</v>
-      </c>
-      <c r="F7" s="10">
-        <v>1</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" t="s" s="10">
-        <v>86</v>
-      </c>
-      <c r="I7" t="s" s="3">
-        <v>22</v>
-      </c>
     </row>
     <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="33"/>
     </row>
     <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
     </row>
     <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="36"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="7.875" defaultRowHeight="14.25" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="7.875" style="37" customWidth="1"/>
+    <col min="2" max="2" width="7.875" style="37" customWidth="1"/>
+    <col min="3" max="3" width="7.875" style="37" customWidth="1"/>
+    <col min="4" max="4" width="7.875" style="37" customWidth="1"/>
+    <col min="5" max="5" width="7.875" style="37" customWidth="1"/>
+    <col min="6" max="256" width="7.875" style="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="19" customHeight="1">
+      <c r="A1" s="38"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+    </row>
+    <row r="2" ht="19" customHeight="1">
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+    </row>
+    <row r="3" ht="19" customHeight="1">
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+    </row>
+    <row r="4" ht="19" customHeight="1">
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+    </row>
+    <row r="5" ht="19" customHeight="1">
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+    </row>
+    <row r="6" ht="19" customHeight="1">
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+    </row>
+    <row r="7" ht="19" customHeight="1">
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+    </row>
+    <row r="8" ht="19" customHeight="1">
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+    </row>
+    <row r="9" ht="19" customHeight="1">
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+    </row>
+    <row r="10" ht="19" customHeight="1">
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>